<commit_message>
rimessa in funzione la simulazione delle elezioni dell'Emilia-Romagna
</commit_message>
<xml_diff>
--- a/scenari/BO_insieme.xlsx
+++ b/scenari/BO_insieme.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\forna\Repos\elezioni-EMR\scenari\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8BAA22-0B6D-4A27-A9FF-57CB29E4C157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1440111-15E2-4722-BF12-15B758FA62C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="liste_future" sheetId="1" r:id="rId1"/>
@@ -734,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -869,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1522,7 +1522,7 @@
         <v>39</v>
       </c>
       <c r="D38" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -2355,7 +2355,7 @@
         <v>71</v>
       </c>
       <c r="D87" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="E87">
         <v>1</v>

</xml_diff>

<commit_message>
andamento passato, tabella prob comunali
</commit_message>
<xml_diff>
--- a/scenari/BO_insieme.xlsx
+++ b/scenari/BO_insieme.xlsx
@@ -5,23 +5,24 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\forna\Repos\elezioni-EMR\scenari\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\forna\Repos\elezioni\scenari\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1440111-15E2-4722-BF12-15B758FA62C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C97A9A7-6971-49F8-A97A-E85722F79E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="liste_future" sheetId="1" r:id="rId1"/>
     <sheet name="flussi_previsti" sheetId="2" r:id="rId2"/>
+    <sheet name="coalizioni_future" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="106">
   <si>
     <t>LISTA_FUTURA</t>
   </si>
@@ -735,7 +736,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B2" sqref="B2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -869,7 +870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
@@ -2614,4 +2615,54 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE50A56E-82DE-4BE7-A522-922D369890F5}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>